<commit_message>
Agregado CrudUsuarios;Arreglos a CRUDexposiciones
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt/Diagrama de Gantt.xlsx
+++ b/Diagrama de Gantt/Diagrama de Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plays\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\vscode\Museo\museo\Diagrama de Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF76CE-1B87-4282-949D-BC327E9303C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C07E9B-9F8F-4A4E-B2B0-C4148540CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>martes</t>
   </si>
@@ -120,13 +120,25 @@
   </si>
   <si>
     <t>21:30 22:30</t>
+  </si>
+  <si>
+    <t>Sistema Web</t>
+  </si>
+  <si>
+    <t>app movil</t>
+  </si>
+  <si>
+    <t>10:00 - 12:00</t>
+  </si>
+  <si>
+    <t>Estefanía y florencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,19 +180,27 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -230,8 +250,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -651,11 +689,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -665,27 +740,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -695,29 +761,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -725,9 +776,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -743,95 +791,183 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="10" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="10" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="9" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="10" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="9" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="5" fillId="10" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="9" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1113,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AG19"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,640 +1273,864 @@
     <col min="33" max="38" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B2" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="92" t="s">
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="92" t="s">
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="94"/>
-      <c r="V2" s="92" t="s">
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="93"/>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="94"/>
-      <c r="AB2" s="92" t="s">
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="93"/>
-      <c r="AE2" s="93"/>
-      <c r="AF2" s="93"/>
-      <c r="AG2" s="94"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="79"/>
     </row>
-    <row r="3" spans="2:33" s="3" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="91"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="75" t="s">
+    <row r="3" spans="1:33" s="3" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="76"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="75" t="s">
+      <c r="J3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="76" t="s">
+      <c r="N3" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="85" t="s">
+      <c r="O3" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="75" t="s">
+      <c r="P3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="76" t="s">
+      <c r="Q3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="76" t="s">
+      <c r="R3" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="76" t="s">
+      <c r="S3" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="76" t="s">
+      <c r="T3" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="77" t="s">
+      <c r="U3" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="75" t="s">
+      <c r="V3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="76" t="s">
+      <c r="W3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="76" t="s">
+      <c r="X3" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="76" t="s">
+      <c r="Y3" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="76" t="s">
+      <c r="Z3" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="76" t="s">
+      <c r="AA3" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="75" t="s">
+      <c r="AB3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="76" t="s">
+      <c r="AC3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="76" t="s">
+      <c r="AD3" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="AE3" s="76" t="s">
+      <c r="AE3" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="76" t="s">
+      <c r="AF3" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="AG3" s="77" t="s">
+      <c r="AG3" s="63" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="95">
         <v>3</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="21"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="18"/>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="89"/>
+      <c r="B5" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="96">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="17"/>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="22"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="19"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="89"/>
+      <c r="B6" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="96">
         <v>2</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="17"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="17"/>
-      <c r="AG6" s="22"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="19"/>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="89"/>
+      <c r="B7" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="96">
         <v>1</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="31"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="17"/>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="22"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="19"/>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
+      <c r="B8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="97">
         <v>2</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="17"/>
-      <c r="AD8" s="17"/>
-      <c r="AE8" s="17"/>
-      <c r="AF8" s="17"/>
-      <c r="AG8" s="22"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="23"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="19"/>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="89"/>
+      <c r="B9" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="96">
         <v>1</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="17"/>
-      <c r="AD9" s="17"/>
-      <c r="AE9" s="17"/>
-      <c r="AF9" s="17"/>
-      <c r="AG9" s="22"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="44"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="19"/>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="89"/>
+      <c r="B10" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="96">
         <v>2</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="17"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="17"/>
-      <c r="AD10" s="17"/>
-      <c r="AE10" s="17"/>
-      <c r="AF10" s="17"/>
-      <c r="AG10" s="22"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="19"/>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="89"/>
+      <c r="B11" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="98">
         <v>14</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
-      <c r="T11" s="58"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="60"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="58"/>
-      <c r="Y11" s="58"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="59"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="58"/>
-      <c r="AD11" s="58"/>
-      <c r="AE11" s="58"/>
-      <c r="AF11" s="58"/>
-      <c r="AG11" s="59"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="46"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="46"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="45"/>
+      <c r="AD11" s="45"/>
+      <c r="AE11" s="45"/>
+      <c r="AF11" s="45"/>
+      <c r="AG11" s="46"/>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="89"/>
+      <c r="B12" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="96">
         <v>14</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="61"/>
-      <c r="S12" s="61"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="62"/>
-      <c r="AC12" s="61"/>
-      <c r="AD12" s="61"/>
-      <c r="AE12" s="61"/>
-      <c r="AF12" s="61"/>
-      <c r="AG12" s="63"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="48"/>
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="50"/>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="37" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="89"/>
+      <c r="B13" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="99">
         <v>14</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="65"/>
-      <c r="W13" s="64"/>
-      <c r="X13" s="64"/>
-      <c r="Y13" s="64"/>
-      <c r="Z13" s="64"/>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="65"/>
-      <c r="AC13" s="64"/>
-      <c r="AD13" s="64"/>
-      <c r="AE13" s="64"/>
-      <c r="AF13" s="64"/>
-      <c r="AG13" s="66"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="51"/>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="51"/>
+      <c r="Z13" s="51"/>
+      <c r="AA13" s="53"/>
+      <c r="AB13" s="52"/>
+      <c r="AC13" s="51"/>
+      <c r="AD13" s="51"/>
+      <c r="AE13" s="51"/>
+      <c r="AF13" s="51"/>
+      <c r="AG13" s="53"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="89"/>
+      <c r="B14" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="100">
         <v>2</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="40"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="31"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="80"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="15"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="66"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="12"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="15"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="12"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="84"/>
-      <c r="AC14" s="78"/>
-      <c r="AD14" s="78"/>
-      <c r="AE14" s="78"/>
-      <c r="AF14" s="78"/>
-      <c r="AG14" s="79"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="70"/>
+      <c r="AC14" s="64"/>
+      <c r="AD14" s="64"/>
+      <c r="AE14" s="64"/>
+      <c r="AF14" s="64"/>
+      <c r="AG14" s="65"/>
     </row>
-    <row r="15" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="93"/>
+      <c r="B15" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="101">
         <v>6</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="36"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="41"/>
-      <c r="AG15" s="36"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="32"/>
+      <c r="AG15" s="28"/>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B16" s="51" t="s">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="98">
+        <v>2</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="109" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="110"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="102"/>
+      <c r="V16" s="103"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="55"/>
+      <c r="Z16" s="55"/>
+      <c r="AA16" s="102"/>
+      <c r="AB16" s="103"/>
+      <c r="AC16" s="55"/>
+      <c r="AD16" s="55"/>
+      <c r="AE16" s="55"/>
+      <c r="AF16" s="55"/>
+      <c r="AG16" s="102"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" s="82"/>
+      <c r="B17" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="96">
+        <v>2</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="111" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="103"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
+      <c r="Y17" s="55"/>
+      <c r="Z17" s="55"/>
+      <c r="AA17" s="102"/>
+      <c r="AB17" s="103"/>
+      <c r="AC17" s="55"/>
+      <c r="AD17" s="55"/>
+      <c r="AE17" s="55"/>
+      <c r="AF17" s="55"/>
+      <c r="AG17" s="102"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" s="82"/>
+      <c r="B18" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="99">
+        <v>2</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="113" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="114"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="104"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="104"/>
+      <c r="AB18" s="105"/>
+      <c r="AC18" s="57"/>
+      <c r="AD18" s="57"/>
+      <c r="AE18" s="57"/>
+      <c r="AF18" s="57"/>
+      <c r="AG18" s="104"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" s="82"/>
+      <c r="B19" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="100">
+        <v>2</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="106"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="W19" s="116"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="70"/>
+      <c r="AC19" s="64"/>
+      <c r="AD19" s="64"/>
+      <c r="AE19" s="64"/>
+      <c r="AF19" s="64"/>
+      <c r="AG19" s="65"/>
+    </row>
+    <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="85"/>
+      <c r="B20" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="101">
+        <v>2</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="117" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC20" s="118"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="32"/>
+      <c r="AG20" s="28"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B22" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C22" s="74" t="s">
         <v>21</v>
       </c>
+      <c r="D22" s="119" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="119"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="s">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="89"/>
-      <c r="D17" s="50"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
     </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="52" t="s">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B24" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
+      <c r="C24" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C16:C18"/>
+  <mergeCells count="15">
+    <mergeCell ref="A4:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="C22:C24"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="AB2:AG2"/>
     <mergeCell ref="V2:AA2"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="D2:I2"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="D22:E23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>